<commit_message>
Add yecc figures and updated report
</commit_message>
<xml_diff>
--- a/Fig_tab_map/external/tables.xlsx
+++ b/Fig_tab_map/external/tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
   </bookViews>
   <sheets>
     <sheet name="table_1" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="68">
   <si>
     <t>Target</t>
   </si>
@@ -64,30 +64,6 @@
     <t>Various emissions targets for 2030</t>
   </si>
   <si>
-    <t>Human Development</t>
-  </si>
-  <si>
-    <t>growth</t>
-  </si>
-  <si>
-    <t>Demographics</t>
-  </si>
-  <si>
-    <t>Scenario 4</t>
-  </si>
-  <si>
-    <t>Scenario 3</t>
-  </si>
-  <si>
-    <t>Scenario 2</t>
-  </si>
-  <si>
-    <t>Scenario 1</t>
-  </si>
-  <si>
-    <t>Scenario</t>
-  </si>
-  <si>
     <t>Stakeholder workshop</t>
   </si>
   <si>
@@ -242,6 +218,18 @@
   </si>
   <si>
     <t>Assume same value for 2050 and assume small ruminants double</t>
+  </si>
+  <si>
+    <t>study</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Objective</t>
+  </si>
+  <si>
+    <t>Climate change</t>
   </si>
 </sst>
 </file>
@@ -577,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,36 +578,18 @@
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -631,7 +601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -650,7 +620,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -658,35 +628,35 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -697,10 +667,10 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -711,10 +681,10 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -725,7 +695,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -736,18 +706,18 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -755,13 +725,13 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -788,13 +758,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -802,133 +772,133 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add updated full report
</commit_message>
<xml_diff>
--- a/Fig_tab_map/external/tables.xlsx
+++ b/Fig_tab_map/external/tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vandijkm\Github\CSIP_ZMB\Fig_tab_map\external\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6A5C32-8F17-4701-B966-FC25E6D1484F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0690CBE-29A1-49D7-B0A9-E2A4D40A2355}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="9735" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="9735" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_1" sheetId="2" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="old_table_2" sheetId="12" r:id="rId4"/>
     <sheet name="table_3" sheetId="11" r:id="rId5"/>
     <sheet name="table_4" sheetId="13" r:id="rId6"/>
+    <sheet name="table_mitt" sheetId="14" r:id="rId7"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="94">
   <si>
     <t>Target</t>
   </si>
@@ -305,6 +306,18 @@
   </si>
   <si>
     <t>Beans (40%),   cassava (17%), chickpeas (90%), cotton (60%), groundnuts (43%), maize (24%), rice (61%),  soya (45%)</t>
+  </si>
+  <si>
+    <t>LUC_Ag</t>
+  </si>
+  <si>
+    <t>LUC_Crp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carbon taxes are applied on emissions from deforestation. Carbon taxes are also applied to the emissions from conversion of natural land to cropland or grassland in Zambia. Emissions from converting grassland to cropland are not taxed. This scenario reflects a holistic policy on LUC targeting all agricultural area. </t>
+  </si>
+  <si>
+    <t>Carbon taxes are applied on emissions from deforestation. Carbon taxes are also applied to emissions from the conversion of grassland to cropland and from natural land to cropland in Zambia. Emissions from the conversion of natural land to grassland are not taxed. This scenario reflects a targeted policy on LUC from only cropland expansion.</t>
   </si>
 </sst>
 </file>
@@ -373,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -407,6 +420,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -696,6 +712,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -1111,7 +1128,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1331,4 +1348,40 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1ABEF9F-EBE5-44C5-BD51-8DD9B391A100}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45.28515625" customWidth="1"/>
+    <col min="2" max="2" width="63.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>